<commit_message>
Fix 1.0.2 (Save as Type Into, Environment.CurrDir)
</commit_message>
<xml_diff>
--- a/Operating Unit.xlsx
+++ b/Operating Unit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\escorpip\Downloads\24. Month End Close 1\24. Month End Close\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\escorpip\ELS_P2P_InvoiceProcessing_MonthEndClose\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C1B67C-6BA1-4847-95A4-73844822EEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E4086D-9154-4CB9-B06D-EA0BFFF7ACB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BEA64C67-C214-4F01-B5D3-63C181DC5500}"/>
   </bookViews>
@@ -601,8 +601,47 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
+      <c r="B2" s="1">
+        <v>45625.785821759258</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45625.788321759261</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45625.790902777779</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45625.795115740744</v>
+      </c>
       <c r="F2" t="s">
         <v>42</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45625.816770833335</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45625.818437499998</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45625.819988425923</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45625.821527777778</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45625.823217592595</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45625.824803240743</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45625.826226851852</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45625.828668981485</v>
+      </c>
+      <c r="O2" s="1">
+        <v>45625.829108796293</v>
       </c>
       <c r="P2">
         <v>701</v>

</xml_diff>